<commit_message>
Added extraction of delivery data
</commit_message>
<xml_diff>
--- a/data/EXP Feb 2018.xlsx
+++ b/data/EXP Feb 2018.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kronos\Dropbox\SMU\Schoolwork\Year 3 Term 2\Enterprise Analytics for Decision Support\Project\EADSProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kronos\Dropbox\SMU\Schoolwork\Year 3 Term 2\Enterprise Analytics for Decision Support\Project\EADSProject\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9285"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7485" windowHeight="6585"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1953,8 +1953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AF10" sqref="AF10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>